<commit_message>
Added new US data
</commit_message>
<xml_diff>
--- a/source-data/britain/britain_covid_source_latest.xlsx
+++ b/source-data/britain/britain_covid_source_latest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamestozer/Documents/GitHub/covid-19-excess-deaths-tracker/source-data/britain/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE498A0E-20D8-544B-AF3F-0502AFC91764}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA997F44-7733-5C47-8E5C-72C32714A33D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="460" windowWidth="19720" windowHeight="15020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7340" yWindow="900" windowWidth="19720" windowHeight="15020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="britain_covid_source_latest" sheetId="1" r:id="rId1"/>
@@ -402,8 +402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G269" workbookViewId="0">
-      <selection activeCell="P276" sqref="P276"/>
+    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
+      <selection activeCell="P280" sqref="P280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -15166,7 +15166,7 @@
         <v>0</v>
       </c>
       <c r="R259">
-        <f t="shared" ref="R259:R286" si="4">SUM(E259,P259:Q259)</f>
+        <f t="shared" ref="R259:R288" si="4">SUM(E259,P259:Q259)</f>
         <v>0</v>
       </c>
     </row>
@@ -16699,14 +16699,14 @@
         <v>57</v>
       </c>
       <c r="P286">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="Q286">
         <v>21</v>
       </c>
       <c r="R286">
         <f t="shared" si="4"/>
-        <v>1184</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="287" spans="1:18">
@@ -16722,6 +16722,49 @@
       <c r="D287">
         <v>25</v>
       </c>
+      <c r="E287">
+        <v>783</v>
+      </c>
+      <c r="F287">
+        <v>30</v>
+      </c>
+      <c r="G287">
+        <v>134</v>
+      </c>
+      <c r="H287">
+        <v>111</v>
+      </c>
+      <c r="I287">
+        <v>96</v>
+      </c>
+      <c r="J287">
+        <v>93</v>
+      </c>
+      <c r="K287">
+        <v>77</v>
+      </c>
+      <c r="L287">
+        <v>50</v>
+      </c>
+      <c r="M287">
+        <v>117</v>
+      </c>
+      <c r="N287">
+        <v>36</v>
+      </c>
+      <c r="O287">
+        <v>39</v>
+      </c>
+      <c r="P287">
+        <v>49</v>
+      </c>
+      <c r="Q287">
+        <v>17</v>
+      </c>
+      <c r="R287">
+        <f t="shared" si="4"/>
+        <v>849</v>
+      </c>
     </row>
     <row r="288" spans="1:18">
       <c r="A288" t="s">
@@ -16735,6 +16778,49 @@
       </c>
       <c r="D288">
         <v>26</v>
+      </c>
+      <c r="E288">
+        <v>606</v>
+      </c>
+      <c r="F288">
+        <v>32</v>
+      </c>
+      <c r="G288">
+        <v>120</v>
+      </c>
+      <c r="H288">
+        <v>69</v>
+      </c>
+      <c r="I288">
+        <v>89</v>
+      </c>
+      <c r="J288">
+        <v>69</v>
+      </c>
+      <c r="K288">
+        <v>59</v>
+      </c>
+      <c r="L288">
+        <v>35</v>
+      </c>
+      <c r="M288">
+        <v>85</v>
+      </c>
+      <c r="N288">
+        <v>16</v>
+      </c>
+      <c r="O288">
+        <v>30</v>
+      </c>
+      <c r="P288">
+        <v>35</v>
+      </c>
+      <c r="Q288">
+        <v>12</v>
+      </c>
+      <c r="R288">
+        <f t="shared" si="4"/>
+        <v>653</v>
       </c>
     </row>
     <row r="289" spans="1:4">

</xml_diff>

<commit_message>
Updated sources and added modelled baselines
</commit_message>
<xml_diff>
--- a/source-data/britain/britain_covid_source_latest.xlsx
+++ b/source-data/britain/britain_covid_source_latest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamestozer/Documents/GitHub/covid-19-excess-deaths-tracker/source-data/britain/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD129114-E2F9-424A-900B-22148167EE55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0075B2F5-4ACA-0D43-9CCC-D5E6E7028462}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="1200" windowWidth="19720" windowHeight="15020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5740" yWindow="580" windowWidth="19720" windowHeight="15020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="britain_covid_source_latest" sheetId="1" r:id="rId1"/>
@@ -88,7 +88,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -402,13 +402,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A272" workbookViewId="0">
-      <selection activeCell="H287" sqref="H287"/>
+    <sheetView tabSelected="1" topLeftCell="A279" workbookViewId="0">
+      <selection activeCell="I292" sqref="I292"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,7 +464,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -521,7 +521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -578,7 +578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -635,7 +635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -692,7 +692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -749,7 +749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -806,7 +806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -863,7 +863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -920,7 +920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -977,7 +977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:18">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:18">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:18">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:18">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -2630,7 +2630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:18">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>17</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:18">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>17</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:18">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:18">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>17</v>
       </c>
@@ -2858,7 +2858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:18">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:18">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:18">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>17</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:18">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>17</v>
       </c>
@@ -3086,7 +3086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:18">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:18">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>17</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:18">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -3257,7 +3257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:18">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>17</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:18">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>17</v>
       </c>
@@ -3371,7 +3371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:18">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>17</v>
       </c>
@@ -3428,7 +3428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:18">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>17</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:18">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>17</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:18">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>17</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:18">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>17</v>
       </c>
@@ -3656,7 +3656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:18">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>17</v>
       </c>
@@ -3713,7 +3713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:18">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>17</v>
       </c>
@@ -3770,7 +3770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:18">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>17</v>
       </c>
@@ -3827,7 +3827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:18">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>17</v>
       </c>
@@ -3884,7 +3884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:18">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>17</v>
       </c>
@@ -3941,7 +3941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:18">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>17</v>
       </c>
@@ -3998,7 +3998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:18">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>17</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:18">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>17</v>
       </c>
@@ -4112,7 +4112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:18">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>17</v>
       </c>
@@ -4169,7 +4169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:18">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>17</v>
       </c>
@@ -4226,7 +4226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:18">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>17</v>
       </c>
@@ -4283,7 +4283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:18">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>17</v>
       </c>
@@ -4340,7 +4340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:18">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>17</v>
       </c>
@@ -4397,7 +4397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:18">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>17</v>
       </c>
@@ -4454,7 +4454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:18">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>17</v>
       </c>
@@ -4511,7 +4511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:18">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>17</v>
       </c>
@@ -4568,7 +4568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:18">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>17</v>
       </c>
@@ -4625,7 +4625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:18">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>17</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:18">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>17</v>
       </c>
@@ -4739,7 +4739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:18">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>17</v>
       </c>
@@ -4796,7 +4796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:18">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>17</v>
       </c>
@@ -4853,7 +4853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:18">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>17</v>
       </c>
@@ -4910,7 +4910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:18">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>17</v>
       </c>
@@ -4967,7 +4967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:18">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>17</v>
       </c>
@@ -5024,7 +5024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:18">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>17</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:18">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>17</v>
       </c>
@@ -5138,7 +5138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:18">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>17</v>
       </c>
@@ -5195,7 +5195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:18">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>17</v>
       </c>
@@ -5252,7 +5252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:18">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>17</v>
       </c>
@@ -5309,7 +5309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:18">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>17</v>
       </c>
@@ -5366,7 +5366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:18">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>17</v>
       </c>
@@ -5423,7 +5423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:18">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>17</v>
       </c>
@@ -5480,7 +5480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:18">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>17</v>
       </c>
@@ -5537,7 +5537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:18">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>17</v>
       </c>
@@ -5594,7 +5594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:18">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>17</v>
       </c>
@@ -5651,7 +5651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:18">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>17</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:18">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>17</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:18">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>17</v>
       </c>
@@ -5822,7 +5822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:18">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>17</v>
       </c>
@@ -5879,7 +5879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:18">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>17</v>
       </c>
@@ -5936,7 +5936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:18">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>17</v>
       </c>
@@ -5993,7 +5993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:18">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>17</v>
       </c>
@@ -6050,7 +6050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:18">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>17</v>
       </c>
@@ -6107,7 +6107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:18">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>17</v>
       </c>
@@ -6164,7 +6164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:18">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>17</v>
       </c>
@@ -6221,7 +6221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:18">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>17</v>
       </c>
@@ -6278,7 +6278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:18">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>17</v>
       </c>
@@ -6335,7 +6335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:18">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>17</v>
       </c>
@@ -6392,7 +6392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:18">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>17</v>
       </c>
@@ -6449,7 +6449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:18">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>17</v>
       </c>
@@ -6506,7 +6506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:18">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>17</v>
       </c>
@@ -6563,7 +6563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:18">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>17</v>
       </c>
@@ -6620,7 +6620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:18">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>17</v>
       </c>
@@ -6677,7 +6677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:18">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>17</v>
       </c>
@@ -6734,7 +6734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:18">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>17</v>
       </c>
@@ -6791,7 +6791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:18">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>17</v>
       </c>
@@ -6848,7 +6848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:18">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>17</v>
       </c>
@@ -6905,7 +6905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:18">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>17</v>
       </c>
@@ -6962,7 +6962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:18">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>17</v>
       </c>
@@ -7019,7 +7019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:18">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>17</v>
       </c>
@@ -7076,7 +7076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:18">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>17</v>
       </c>
@@ -7133,7 +7133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:18">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>17</v>
       </c>
@@ -7190,7 +7190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:18">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>17</v>
       </c>
@@ -7247,7 +7247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:18">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>17</v>
       </c>
@@ -7304,7 +7304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:18">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>17</v>
       </c>
@@ -7361,7 +7361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:18">
+    <row r="123" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>17</v>
       </c>
@@ -7418,7 +7418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:18">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>17</v>
       </c>
@@ -7475,7 +7475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:18">
+    <row r="125" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>17</v>
       </c>
@@ -7532,7 +7532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:18">
+    <row r="126" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>17</v>
       </c>
@@ -7589,7 +7589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:18">
+    <row r="127" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>17</v>
       </c>
@@ -7646,7 +7646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:18">
+    <row r="128" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>17</v>
       </c>
@@ -7703,7 +7703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:18">
+    <row r="129" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>17</v>
       </c>
@@ -7760,7 +7760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:18">
+    <row r="130" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>17</v>
       </c>
@@ -7817,7 +7817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:18">
+    <row r="131" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>17</v>
       </c>
@@ -7874,7 +7874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:18">
+    <row r="132" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>17</v>
       </c>
@@ -7931,7 +7931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:18">
+    <row r="133" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>17</v>
       </c>
@@ -7988,7 +7988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:18">
+    <row r="134" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>17</v>
       </c>
@@ -8045,7 +8045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:18">
+    <row r="135" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>17</v>
       </c>
@@ -8102,7 +8102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:18">
+    <row r="136" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>17</v>
       </c>
@@ -8159,7 +8159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:18">
+    <row r="137" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>17</v>
       </c>
@@ -8216,7 +8216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:18">
+    <row r="138" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>17</v>
       </c>
@@ -8273,7 +8273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:18">
+    <row r="139" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>17</v>
       </c>
@@ -8330,7 +8330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:18">
+    <row r="140" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>17</v>
       </c>
@@ -8387,7 +8387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:18">
+    <row r="141" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>17</v>
       </c>
@@ -8444,7 +8444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:18">
+    <row r="142" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>17</v>
       </c>
@@ -8501,7 +8501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:18">
+    <row r="143" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>17</v>
       </c>
@@ -8558,7 +8558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:18">
+    <row r="144" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>17</v>
       </c>
@@ -8615,7 +8615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:18">
+    <row r="145" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>17</v>
       </c>
@@ -8672,7 +8672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:18">
+    <row r="146" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>17</v>
       </c>
@@ -8729,7 +8729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:18">
+    <row r="147" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>17</v>
       </c>
@@ -8786,7 +8786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:18">
+    <row r="148" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>17</v>
       </c>
@@ -8843,7 +8843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:18">
+    <row r="149" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>17</v>
       </c>
@@ -8900,7 +8900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:18">
+    <row r="150" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>17</v>
       </c>
@@ -8957,7 +8957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:18">
+    <row r="151" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>17</v>
       </c>
@@ -9014,7 +9014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:18">
+    <row r="152" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>17</v>
       </c>
@@ -9071,7 +9071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:18">
+    <row r="153" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>17</v>
       </c>
@@ -9128,7 +9128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:18">
+    <row r="154" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>17</v>
       </c>
@@ -9185,7 +9185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:18">
+    <row r="155" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>17</v>
       </c>
@@ -9242,7 +9242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:18">
+    <row r="156" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>17</v>
       </c>
@@ -9299,7 +9299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:18">
+    <row r="157" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>17</v>
       </c>
@@ -9356,7 +9356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:18">
+    <row r="158" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>17</v>
       </c>
@@ -9413,7 +9413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:18">
+    <row r="159" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>17</v>
       </c>
@@ -9470,7 +9470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:18">
+    <row r="160" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>17</v>
       </c>
@@ -9527,7 +9527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:18">
+    <row r="161" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>17</v>
       </c>
@@ -9584,7 +9584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:18">
+    <row r="162" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>17</v>
       </c>
@@ -9641,7 +9641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:18">
+    <row r="163" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>17</v>
       </c>
@@ -9698,7 +9698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:18">
+    <row r="164" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>17</v>
       </c>
@@ -9755,7 +9755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:18">
+    <row r="165" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>17</v>
       </c>
@@ -9812,7 +9812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:18">
+    <row r="166" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>17</v>
       </c>
@@ -9869,7 +9869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:18">
+    <row r="167" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>17</v>
       </c>
@@ -9926,7 +9926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:18">
+    <row r="168" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>17</v>
       </c>
@@ -9983,7 +9983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:18">
+    <row r="169" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>17</v>
       </c>
@@ -10040,7 +10040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:18">
+    <row r="170" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>17</v>
       </c>
@@ -10097,7 +10097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:18">
+    <row r="171" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>17</v>
       </c>
@@ -10154,7 +10154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:18">
+    <row r="172" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>17</v>
       </c>
@@ -10211,7 +10211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:18">
+    <row r="173" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>17</v>
       </c>
@@ -10268,7 +10268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:18">
+    <row r="174" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>17</v>
       </c>
@@ -10325,7 +10325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:18">
+    <row r="175" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>17</v>
       </c>
@@ -10382,7 +10382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:18">
+    <row r="176" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>17</v>
       </c>
@@ -10439,7 +10439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:18">
+    <row r="177" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>17</v>
       </c>
@@ -10496,7 +10496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:18">
+    <row r="178" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>17</v>
       </c>
@@ -10553,7 +10553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:18">
+    <row r="179" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>17</v>
       </c>
@@ -10610,7 +10610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:18">
+    <row r="180" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>17</v>
       </c>
@@ -10667,7 +10667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:18">
+    <row r="181" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>17</v>
       </c>
@@ -10724,7 +10724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:18">
+    <row r="182" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>17</v>
       </c>
@@ -10781,7 +10781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:18">
+    <row r="183" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>17</v>
       </c>
@@ -10838,7 +10838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:18">
+    <row r="184" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>17</v>
       </c>
@@ -10895,7 +10895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:18">
+    <row r="185" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>17</v>
       </c>
@@ -10952,7 +10952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:18">
+    <row r="186" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>17</v>
       </c>
@@ -11009,7 +11009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:18">
+    <row r="187" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>17</v>
       </c>
@@ -11066,7 +11066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:18">
+    <row r="188" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>17</v>
       </c>
@@ -11123,7 +11123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:18">
+    <row r="189" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>17</v>
       </c>
@@ -11180,7 +11180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:18">
+    <row r="190" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>17</v>
       </c>
@@ -11237,7 +11237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:18">
+    <row r="191" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>17</v>
       </c>
@@ -11294,7 +11294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:18">
+    <row r="192" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>17</v>
       </c>
@@ -11351,7 +11351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:18">
+    <row r="193" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>17</v>
       </c>
@@ -11408,7 +11408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:18">
+    <row r="194" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>17</v>
       </c>
@@ -11465,7 +11465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:18">
+    <row r="195" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>17</v>
       </c>
@@ -11522,7 +11522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:18">
+    <row r="196" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>17</v>
       </c>
@@ -11579,7 +11579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:18">
+    <row r="197" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>17</v>
       </c>
@@ -11636,7 +11636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:18">
+    <row r="198" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>17</v>
       </c>
@@ -11693,7 +11693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:18">
+    <row r="199" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>17</v>
       </c>
@@ -11750,7 +11750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:18">
+    <row r="200" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>17</v>
       </c>
@@ -11807,7 +11807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:18">
+    <row r="201" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>17</v>
       </c>
@@ -11864,7 +11864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:18">
+    <row r="202" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>17</v>
       </c>
@@ -11921,7 +11921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:18">
+    <row r="203" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>17</v>
       </c>
@@ -11978,7 +11978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:18">
+    <row r="204" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>17</v>
       </c>
@@ -12035,7 +12035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:18">
+    <row r="205" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>17</v>
       </c>
@@ -12092,7 +12092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:18">
+    <row r="206" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>17</v>
       </c>
@@ -12149,7 +12149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:18">
+    <row r="207" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>17</v>
       </c>
@@ -12206,7 +12206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:18">
+    <row r="208" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>17</v>
       </c>
@@ -12263,7 +12263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:18">
+    <row r="209" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>17</v>
       </c>
@@ -12320,7 +12320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:18">
+    <row r="210" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>17</v>
       </c>
@@ -12377,7 +12377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:18">
+    <row r="211" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>17</v>
       </c>
@@ -12434,7 +12434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:18">
+    <row r="212" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>17</v>
       </c>
@@ -12491,7 +12491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:18">
+    <row r="213" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>17</v>
       </c>
@@ -12548,7 +12548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:18">
+    <row r="214" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>17</v>
       </c>
@@ -12605,7 +12605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:18">
+    <row r="215" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>17</v>
       </c>
@@ -12662,7 +12662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:18">
+    <row r="216" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>17</v>
       </c>
@@ -12719,7 +12719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:18">
+    <row r="217" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>17</v>
       </c>
@@ -12776,7 +12776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:18">
+    <row r="218" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>17</v>
       </c>
@@ -12833,7 +12833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:18">
+    <row r="219" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>17</v>
       </c>
@@ -12890,7 +12890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:18">
+    <row r="220" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>17</v>
       </c>
@@ -12947,7 +12947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:18">
+    <row r="221" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>17</v>
       </c>
@@ -13004,7 +13004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:18">
+    <row r="222" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>17</v>
       </c>
@@ -13061,7 +13061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:18">
+    <row r="223" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>17</v>
       </c>
@@ -13118,7 +13118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:18">
+    <row r="224" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>17</v>
       </c>
@@ -13175,7 +13175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:18">
+    <row r="225" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>17</v>
       </c>
@@ -13232,7 +13232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:18">
+    <row r="226" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>17</v>
       </c>
@@ -13289,7 +13289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:18">
+    <row r="227" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>17</v>
       </c>
@@ -13346,7 +13346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:18">
+    <row r="228" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>17</v>
       </c>
@@ -13403,7 +13403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:18">
+    <row r="229" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>17</v>
       </c>
@@ -13460,7 +13460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:18">
+    <row r="230" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>17</v>
       </c>
@@ -13517,7 +13517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:18">
+    <row r="231" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>17</v>
       </c>
@@ -13574,7 +13574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:18">
+    <row r="232" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>17</v>
       </c>
@@ -13631,7 +13631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:18">
+    <row r="233" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>17</v>
       </c>
@@ -13688,7 +13688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:18">
+    <row r="234" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>17</v>
       </c>
@@ -13745,7 +13745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:18">
+    <row r="235" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>17</v>
       </c>
@@ -13802,7 +13802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:18">
+    <row r="236" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>17</v>
       </c>
@@ -13859,7 +13859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:18">
+    <row r="237" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>17</v>
       </c>
@@ -13916,7 +13916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:18">
+    <row r="238" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>17</v>
       </c>
@@ -13973,7 +13973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:18">
+    <row r="239" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>17</v>
       </c>
@@ -14030,7 +14030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:18">
+    <row r="240" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>17</v>
       </c>
@@ -14087,7 +14087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:18">
+    <row r="241" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>17</v>
       </c>
@@ -14144,7 +14144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:18">
+    <row r="242" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>17</v>
       </c>
@@ -14201,7 +14201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:18">
+    <row r="243" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>17</v>
       </c>
@@ -14258,7 +14258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:18">
+    <row r="244" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>17</v>
       </c>
@@ -14315,7 +14315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:18">
+    <row r="245" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>17</v>
       </c>
@@ -14372,7 +14372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:18">
+    <row r="246" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>17</v>
       </c>
@@ -14429,7 +14429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:18">
+    <row r="247" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>17</v>
       </c>
@@ -14486,7 +14486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:18">
+    <row r="248" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>17</v>
       </c>
@@ -14543,7 +14543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:18">
+    <row r="249" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>17</v>
       </c>
@@ -14600,7 +14600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:18">
+    <row r="250" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>17</v>
       </c>
@@ -14657,7 +14657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:18">
+    <row r="251" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>17</v>
       </c>
@@ -14714,7 +14714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:18">
+    <row r="252" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>17</v>
       </c>
@@ -14771,7 +14771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:18">
+    <row r="253" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>17</v>
       </c>
@@ -14828,7 +14828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:18">
+    <row r="254" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>17</v>
       </c>
@@ -14885,7 +14885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:18">
+    <row r="255" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>17</v>
       </c>
@@ -14942,7 +14942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:18">
+    <row r="256" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>17</v>
       </c>
@@ -14999,7 +14999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:18">
+    <row r="257" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>17</v>
       </c>
@@ -15056,7 +15056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:18">
+    <row r="258" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>17</v>
       </c>
@@ -15113,7 +15113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:18">
+    <row r="259" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>17</v>
       </c>
@@ -15166,11 +15166,11 @@
         <v>0</v>
       </c>
       <c r="R259">
-        <f t="shared" ref="R259:R295" si="4">SUM(E259,P259:Q259)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="260" spans="1:18">
+        <f t="shared" ref="R259:R298" si="4">SUM(E259,P259:Q259)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>17</v>
       </c>
@@ -15227,7 +15227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:18">
+    <row r="261" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>17</v>
       </c>
@@ -15284,7 +15284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:18">
+    <row r="262" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>17</v>
       </c>
@@ -15341,7 +15341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:18">
+    <row r="263" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>17</v>
       </c>
@@ -15398,7 +15398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:18">
+    <row r="264" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>17</v>
       </c>
@@ -15455,7 +15455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:18">
+    <row r="265" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>17</v>
       </c>
@@ -15512,7 +15512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:18">
+    <row r="266" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>17</v>
       </c>
@@ -15569,7 +15569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:18">
+    <row r="267" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>17</v>
       </c>
@@ -15626,7 +15626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:18">
+    <row r="268" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>17</v>
       </c>
@@ -15683,7 +15683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:18">
+    <row r="269" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>17</v>
       </c>
@@ -15740,7 +15740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:18">
+    <row r="270" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>17</v>
       </c>
@@ -15797,7 +15797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:18">
+    <row r="271" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>17</v>
       </c>
@@ -15854,7 +15854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:18">
+    <row r="272" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>17</v>
       </c>
@@ -15911,7 +15911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:18">
+    <row r="273" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>17</v>
       </c>
@@ -15968,7 +15968,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="274" spans="1:18">
+    <row r="274" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>17</v>
       </c>
@@ -16015,17 +16015,17 @@
         <v>2</v>
       </c>
       <c r="P274">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Q274">
         <v>1</v>
       </c>
       <c r="R274">
         <f t="shared" si="4"/>
-        <v>114</v>
-      </c>
-    </row>
-    <row r="275" spans="1:18">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="275" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>17</v>
       </c>
@@ -16082,7 +16082,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="276" spans="1:18">
+    <row r="276" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>17</v>
       </c>
@@ -16139,7 +16139,7 @@
         <v>3812</v>
       </c>
     </row>
-    <row r="277" spans="1:18">
+    <row r="277" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>17</v>
       </c>
@@ -16186,17 +16186,17 @@
         <v>304</v>
       </c>
       <c r="P277">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="Q277">
         <v>76</v>
       </c>
       <c r="R277">
         <f t="shared" si="4"/>
-        <v>6899</v>
-      </c>
-    </row>
-    <row r="278" spans="1:18">
+        <v>6898</v>
+      </c>
+    </row>
+    <row r="278" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>17</v>
       </c>
@@ -16253,7 +16253,7 @@
         <v>9509</v>
       </c>
     </row>
-    <row r="279" spans="1:18">
+    <row r="279" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>17</v>
       </c>
@@ -16300,17 +16300,17 @@
         <v>413</v>
       </c>
       <c r="P279">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="Q279">
         <v>128</v>
       </c>
       <c r="R279">
         <f t="shared" si="4"/>
-        <v>9024</v>
-      </c>
-    </row>
-    <row r="280" spans="1:18">
+        <v>9026</v>
+      </c>
+    </row>
+    <row r="280" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>17</v>
       </c>
@@ -16357,17 +16357,17 @@
         <v>281</v>
       </c>
       <c r="P280">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="Q280">
         <v>124</v>
       </c>
       <c r="R280">
         <f t="shared" si="4"/>
-        <v>6685</v>
-      </c>
-    </row>
-    <row r="281" spans="1:18">
+        <v>6686</v>
+      </c>
+    </row>
+    <row r="281" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>17</v>
       </c>
@@ -16424,7 +16424,7 @@
         <v>4429</v>
       </c>
     </row>
-    <row r="282" spans="1:18">
+    <row r="282" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>17</v>
       </c>
@@ -16481,7 +16481,7 @@
         <v>4220</v>
       </c>
     </row>
-    <row r="283" spans="1:18">
+    <row r="283" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>17</v>
       </c>
@@ -16538,7 +16538,7 @@
         <v>2872</v>
       </c>
     </row>
-    <row r="284" spans="1:18">
+    <row r="284" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>17</v>
       </c>
@@ -16595,7 +16595,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="285" spans="1:18">
+    <row r="285" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>17</v>
       </c>
@@ -16652,7 +16652,7 @@
         <v>1697</v>
       </c>
     </row>
-    <row r="286" spans="1:18">
+    <row r="286" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>17</v>
       </c>
@@ -16709,7 +16709,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="287" spans="1:18">
+    <row r="287" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>17</v>
       </c>
@@ -16766,7 +16766,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="288" spans="1:18">
+    <row r="288" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>17</v>
       </c>
@@ -16823,7 +16823,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="289" spans="1:18">
+    <row r="289" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>17</v>
       </c>
@@ -16880,7 +16880,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="290" spans="1:18">
+    <row r="290" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>17</v>
       </c>
@@ -16937,7 +16937,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="291" spans="1:18">
+    <row r="291" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>17</v>
       </c>
@@ -16994,7 +16994,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="292" spans="1:18">
+    <row r="292" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>17</v>
       </c>
@@ -17051,7 +17051,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="293" spans="1:18">
+    <row r="293" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>17</v>
       </c>
@@ -17108,7 +17108,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="294" spans="1:18">
+    <row r="294" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>17</v>
       </c>
@@ -17165,7 +17165,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="295" spans="1:18">
+    <row r="295" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>17</v>
       </c>
@@ -17222,7 +17222,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="296" spans="1:18">
+    <row r="296" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>17</v>
       </c>
@@ -17235,8 +17235,51 @@
       <c r="D296">
         <v>34</v>
       </c>
-    </row>
-    <row r="297" spans="1:18">
+      <c r="E296">
+        <v>138</v>
+      </c>
+      <c r="F296">
+        <v>4</v>
+      </c>
+      <c r="G296">
+        <v>33</v>
+      </c>
+      <c r="H296">
+        <v>12</v>
+      </c>
+      <c r="I296">
+        <v>21</v>
+      </c>
+      <c r="J296">
+        <v>10</v>
+      </c>
+      <c r="K296">
+        <v>7</v>
+      </c>
+      <c r="L296">
+        <v>10</v>
+      </c>
+      <c r="M296">
+        <v>24</v>
+      </c>
+      <c r="N296">
+        <v>5</v>
+      </c>
+      <c r="O296">
+        <v>11</v>
+      </c>
+      <c r="P296">
+        <v>6</v>
+      </c>
+      <c r="Q296">
+        <v>6</v>
+      </c>
+      <c r="R296">
+        <f t="shared" si="4"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="297" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>17</v>
       </c>
@@ -17249,8 +17292,51 @@
       <c r="D297">
         <v>35</v>
       </c>
-    </row>
-    <row r="298" spans="1:18">
+      <c r="E297">
+        <v>101</v>
+      </c>
+      <c r="F297">
+        <v>2</v>
+      </c>
+      <c r="G297">
+        <v>34</v>
+      </c>
+      <c r="H297">
+        <v>13</v>
+      </c>
+      <c r="I297">
+        <v>6</v>
+      </c>
+      <c r="J297">
+        <v>5</v>
+      </c>
+      <c r="K297">
+        <v>16</v>
+      </c>
+      <c r="L297">
+        <v>4</v>
+      </c>
+      <c r="M297">
+        <v>11</v>
+      </c>
+      <c r="N297">
+        <v>6</v>
+      </c>
+      <c r="O297">
+        <v>3</v>
+      </c>
+      <c r="P297">
+        <v>7</v>
+      </c>
+      <c r="Q297">
+        <v>4</v>
+      </c>
+      <c r="R297">
+        <f t="shared" si="4"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="298" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>17</v>
       </c>
@@ -17263,8 +17349,51 @@
       <c r="D298">
         <v>36</v>
       </c>
-    </row>
-    <row r="299" spans="1:18">
+      <c r="E298">
+        <v>78</v>
+      </c>
+      <c r="F298">
+        <v>5</v>
+      </c>
+      <c r="G298">
+        <v>13</v>
+      </c>
+      <c r="H298">
+        <v>10</v>
+      </c>
+      <c r="I298">
+        <v>10</v>
+      </c>
+      <c r="J298">
+        <v>9</v>
+      </c>
+      <c r="K298">
+        <v>6</v>
+      </c>
+      <c r="L298">
+        <v>2</v>
+      </c>
+      <c r="M298">
+        <v>17</v>
+      </c>
+      <c r="N298">
+        <v>2</v>
+      </c>
+      <c r="O298">
+        <v>4</v>
+      </c>
+      <c r="P298">
+        <v>2</v>
+      </c>
+      <c r="Q298">
+        <v>3</v>
+      </c>
+      <c r="R298">
+        <f t="shared" si="4"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="299" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>17</v>
       </c>
@@ -17278,7 +17407,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="300" spans="1:18">
+    <row r="300" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>17</v>
       </c>
@@ -17292,7 +17421,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="301" spans="1:18">
+    <row r="301" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>17</v>
       </c>
@@ -17306,7 +17435,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="302" spans="1:18">
+    <row r="302" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>17</v>
       </c>
@@ -17320,7 +17449,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="303" spans="1:18">
+    <row r="303" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>17</v>
       </c>
@@ -17334,7 +17463,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="304" spans="1:18">
+    <row r="304" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>17</v>
       </c>
@@ -17348,7 +17477,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="305" spans="1:4">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>17</v>
       </c>
@@ -17362,7 +17491,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="306" spans="1:4">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>17</v>
       </c>
@@ -17376,7 +17505,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="307" spans="1:4">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>17</v>
       </c>
@@ -17390,7 +17519,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="308" spans="1:4">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>17</v>
       </c>
@@ -17404,7 +17533,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="309" spans="1:4">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>17</v>
       </c>
@@ -17418,7 +17547,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="310" spans="1:4">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>17</v>
       </c>
@@ -17432,7 +17561,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="311" spans="1:4">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>17</v>
       </c>
@@ -17446,7 +17575,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="312" spans="1:4">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>17</v>
       </c>
@@ -17460,7 +17589,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="313" spans="1:4">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>17</v>
       </c>
@@ -17474,7 +17603,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="314" spans="1:4">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>17</v>
       </c>
@@ -17488,7 +17617,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="315" spans="1:4">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>17</v>
       </c>

</xml_diff>